<commit_message>
Improved the template for better reporting
</commit_message>
<xml_diff>
--- a/src/test/resources/template/Jmeter_Reporting_Template.xlsx
+++ b/src/test/resources/template/Jmeter_Reporting_Template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john.mathew\workspace_oxygen\meagan\src\test\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478C8648-64D9-45E3-A806-7F072087AA9A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transaction Level" sheetId="1" r:id="rId1"/>
@@ -54,7 +55,7 @@
           </rPr>
           <t xml:space="preserve">
 jx:area(lastCell="C10")
-jx:each(lastCell="C10" items="summarys" var="successSummary")</t>
+jx:each(lastCell="C10" items="summarys1" var="successSummary")</t>
         </r>
       </text>
     </comment>
@@ -78,8 +79,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="L10000")
-jx:each(lastCell="L10000" items="summarys" var="successSummary")</t>
+jx:area(lastCell="L1000000")
+jx:each(lastCell="L1000000" items="summarys1" var="successSummary")</t>
         </r>
       </text>
     </comment>
@@ -113,8 +114,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="L100")
-jx:each(lastCell="L100" items="summarys" var="allSummary")</t>
+jx:area(lastCell="L100000")
+jx:each(lastCell="L100000" items="summarys2" var="allSummary")</t>
         </r>
       </text>
     </comment>
@@ -123,6 +124,41 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>John Mathew</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{C7BA1B10-1EF0-4DF7-BB71-C96B4418F5DB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>John Mathew:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:area(lastCell="B1000")
+jx:each(lastCell="B1000" items="tList" var="t")</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>John Mathew</author>
@@ -148,8 +184,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="L10000")
-jx:each(lastCell="L10000" items="summarys" var="errorSummary")</t>
+jx:area(lastCell="L1000000")
+jx:each(lastCell="L1000000" items="summarys3" var="errorSummary")</t>
         </r>
       </text>
     </comment>
@@ -158,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="68">
   <si>
     <t>Summary</t>
   </si>
@@ -259,75 +295,9 @@
     <t>=====================================</t>
   </si>
   <si>
-    <t>14_EditInternalUser_003_EditUser</t>
-  </si>
-  <si>
-    <t>01_Login_ExternalUser_002_Validate_User</t>
-  </si>
-  <si>
-    <t>15_LoanConditions_002_Validate_User</t>
-  </si>
-  <si>
-    <t>17_UPLOADDocuments__002_Validate_User</t>
-  </si>
-  <si>
-    <t>08_LoanSummary_004_pipelineloans</t>
-  </si>
-  <si>
-    <t>08_LoanSummary_002_Validate_User</t>
-  </si>
-  <si>
-    <t>21_OrderAppraisal_002_Validate_User</t>
-  </si>
-  <si>
-    <t>10_Pricing_002_ValidateUser</t>
-  </si>
-  <si>
-    <t>20_LoanOrderDocs_002_Validate_User</t>
-  </si>
-  <si>
-    <t>07_Script2_ManualRegistrationMaxflow_002_Validate_User</t>
-  </si>
-  <si>
-    <t>18_ViewDocuments_005_BackToPipleLine</t>
-  </si>
-  <si>
-    <t>09_1003Form_002_Validate_User</t>
-  </si>
-  <si>
-    <t>18_ViewDocuments_002_Validate_User</t>
-  </si>
-  <si>
-    <t>07_RegisterLoan_manualRegistratio_002_Validate_User</t>
-  </si>
-  <si>
-    <t>02_Login_InternalUser_002_TavantOneLogin</t>
-  </si>
-  <si>
-    <t>14_EditInternalUser_002_TavantOneLogin</t>
-  </si>
-  <si>
-    <t>12_CreateInternalUser_002_TavantOneLogin</t>
-  </si>
-  <si>
-    <t>13_CreateExternalUser_002_TavantOneLogin</t>
-  </si>
-  <si>
-    <t>11_CompanyUpdate_002_TavantOneLogin</t>
-  </si>
-  <si>
-    <t>03_Pagenation_Page10,20,30_ActiveLoans_002_Validate_User</t>
-  </si>
-  <si>
-    <t>06_RegisterLoan_UploadFNM_002_Validate_User</t>
-  </si>
-  <si>
     <t>Transactions Fall between 10 to 20 Seconds</t>
   </si>
   <si>
-    <t>10_Pricing_003_LoanSummary</t>
-  </si>
-  <si>
     <t>18_ViewDocuments_003_LoanSummary</t>
   </si>
   <si>
@@ -446,6 +416,9 @@
   </si>
   <si>
     <t>Std. Dev.</t>
+  </si>
+  <si>
+    <t>10_Pricing_0+B30:B3703_LoanSummary</t>
   </si>
 </sst>
 </file>
@@ -1596,7 +1569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK136"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1669,7 +1642,7 @@
         <v>4</v>
       </c>
       <c r="G11" s="37" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="H11" s="19" t="s">
         <v>5</v>
@@ -5794,7 +5767,7 @@
   <dimension ref="B1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5829,7 +5802,7 @@
         <v>18</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="I2" s="17" t="s">
         <v>21</v>
@@ -5851,11 +5824,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E02DFAF2-AB79-423A-ACCB-9EDFD585605A}">
-  <dimension ref="B2:B71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E02DFAF2-AB79-423A-ACCB-9EDFD585605A}">
+  <dimension ref="B1:B71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B6" sqref="B6:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5865,6 +5838,7 @@
     <col min="3" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:2" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="12" t="s">
         <v>24</v>
@@ -5876,113 +5850,81 @@
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="16" t="s">
-        <v>26</v>
-      </c>
+      <c r="B5" s="16"/>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="16" t="s">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="23" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="16" t="s">
-        <v>34</v>
-      </c>
-    </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="16" t="s">
-        <v>35</v>
-      </c>
+      <c r="B14" s="16"/>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B15" s="16" t="s">
-        <v>36</v>
-      </c>
+      <c r="B15" s="16"/>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="16" t="s">
-        <v>37</v>
-      </c>
+      <c r="B16" s="16"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="16" t="s">
-        <v>38</v>
-      </c>
+      <c r="B17" s="16"/>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="16" t="s">
-        <v>39</v>
-      </c>
+      <c r="B18" s="16"/>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="16" t="s">
-        <v>40</v>
-      </c>
+      <c r="B19" s="16"/>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="16" t="s">
-        <v>41</v>
-      </c>
+      <c r="B20" s="16"/>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="16" t="s">
-        <v>42</v>
-      </c>
+      <c r="B21" s="16"/>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="16" t="s">
-        <v>43</v>
-      </c>
+      <c r="B22" s="16"/>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="8" t="s">
-        <v>46</v>
-      </c>
+      <c r="B23" s="16"/>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
@@ -5992,52 +5934,52 @@
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="23" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="23" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" s="23" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="23" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="23" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="23" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="23" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="23" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="23" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="23" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
@@ -6051,7 +5993,7 @@
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" s="10" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
@@ -6061,37 +6003,37 @@
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" s="16" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" s="16" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" s="16" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="16" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="16" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="8" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" s="10" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
@@ -6101,77 +6043,78 @@
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" s="16" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="16" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="16" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" s="16" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" s="16" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" s="16" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" s="16" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="16" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="16" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" s="16" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" s="16" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
     </row>
     <row r="69" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B69" s="16" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" s="8" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" s="8" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6179,8 +6122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F365DCCC-F353-4CFC-BF73-ACC82FEB2F4F}">
   <dimension ref="B4:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6202,25 +6145,25 @@
         <v>16</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="F5" s="28" t="s">
         <v>18</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="H5" s="28" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="I5" s="28" t="s">
         <v>21</v>
       </c>
       <c r="J5" s="28" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="K5" s="29" t="s">
         <v>23</v>
@@ -6375,10 +6318,10 @@
     <row r="22" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="34" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="C23" s="35" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
removed tList for transaction comparable
</commit_message>
<xml_diff>
--- a/src/test/resources/template/Jmeter_Reporting_Template.xlsx
+++ b/src/test/resources/template/Jmeter_Reporting_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john.mathew\workspace_oxygen\meagan\src\test\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478C8648-64D9-45E3-A806-7F072087AA9A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD690AA-3B6A-4FA1-A6C6-EBC9F65F2E80}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transaction Level" sheetId="1" r:id="rId1"/>
@@ -124,41 +124,6 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>John Mathew</author>
-  </authors>
-  <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{C7BA1B10-1EF0-4DF7-BB71-C96B4418F5DB}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>John Mathew:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:area(lastCell="B1000")
-jx:each(lastCell="B1000" items="tList" var="t")</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>John Mathew</author>
@@ -1569,7 +1534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -5824,11 +5789,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E02DFAF2-AB79-423A-ACCB-9EDFD585605A}">
-  <dimension ref="B1:B71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E02DFAF2-AB79-423A-ACCB-9EDFD585605A}">
+  <dimension ref="B2:B71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5838,7 +5803,6 @@
     <col min="3" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="12" t="s">
         <v>24</v>
@@ -6114,7 +6078,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Improved template to filter Transaction names and Transactions with high response times
</commit_message>
<xml_diff>
--- a/src/test/resources/template/Jmeter_Reporting_Template.xlsx
+++ b/src/test/resources/template/Jmeter_Reporting_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john.mathew\workspace_oxygen\meagan\src\test\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF21343-2B80-4E6D-9635-B6A80FAFFDC4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113B413D-3909-4C95-9EED-89D755B1F3C3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transaction Level" sheetId="1" r:id="rId1"/>
@@ -55,11 +55,11 @@
           </rPr>
           <t xml:space="preserve">
 jx:area(lastCell="C10")
-jx:each(lastCell="C10" items="summarys1" var="successSummary")</t>
+jx:each(lastCell="C10" items="shList" var="sh")</t>
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="1" shapeId="0" xr:uid="{372880A4-EE70-436A-8875-188CA0494723}">
+    <comment ref="B12" authorId="1" shapeId="0" xr:uid="{C4F20104-B0EE-4DB2-AE46-5E8396930D83}">
       <text>
         <r>
           <rPr>
@@ -79,8 +79,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="L1000000")
-jx:each(lastCell="L1000000" items="summarys1" var="successSummary")</t>
+jx:area(lastCell="L12")
+jx:each(lastCell="L12" items="rList1" var="r" select="r.transaction=~'^([0-9]{2,2})+_([0-9]{3,3})+_([A-Za-z])+_([A-Za-z])+$'")</t>
         </r>
       </text>
     </comment>
@@ -94,7 +94,7 @@
     <author>John Mathew</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{449205D4-39CC-40F6-B732-C8BBC247283C}">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{19CF8050-F323-418C-B842-DADBBC95B3B9}">
       <text>
         <r>
           <rPr>
@@ -114,8 +114,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="L100000")
-jx:each(lastCell="L100000" items="summarys2" var="allSummary")</t>
+jx:area(lastCell="L3")
+jx:each(lastCell="L3" items="rList2" var="r")</t>
         </r>
       </text>
     </comment>
@@ -129,7 +129,7 @@
     <author>John Mathew</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{CA5159B3-A8C7-4B80-8D80-2349447B819B}">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{6A90AD79-F00F-4D0C-BEC1-32CBD6C64694}">
       <text>
         <r>
           <rPr>
@@ -149,8 +149,118 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="L1000000")
-jx:each(lastCell="L1000000" items="summarys3" var="errorSummary")</t>
+jx:area(lastCell="B5")
+jx:each(lastCell="B5" items="rList4" var="r" select="r.transaction=~'^([0-9]{2,2})+_([0-9]{3,3})+_([A-Za-z])+_([A-Za-z])+$' and r.averageResponseTime&gt;=5.0 and r.averageResponseTime&lt;10.0")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B31" authorId="0" shapeId="0" xr:uid="{36CBC51F-0211-4A34-ACBB-030D070E157E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>John Mathew:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:area(lastCell="B31")
+jx:each(lastCell="B31" items="rList4" var="r" select="r.transaction=~'^([0-9]{2,2})+_([0-9]{3,3})+_([A-Za-z])+_([A-Za-z])+$' and r.averageResponseTime&gt;=10.0 and r.averageResponseTime&lt;20.0")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B46" authorId="0" shapeId="0" xr:uid="{68E60088-9440-42CF-997B-72FC7A51A7BB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>John Mathew:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:area(lastCell="B46")
+jx:each(lastCell="B46" items="rList4" var="r" select="r.transaction=~'^([0-9]{2,2})+_([0-9]{3,3})+_([A-Za-z])+_([A-Za-z])+$' and r.averageResponseTime&gt;=20.0 and r.averageResponseTime&lt;30.0")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B58" authorId="0" shapeId="0" xr:uid="{B5F5E9F2-2969-4B4A-9D6B-6E3160F39E2A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>John Mathew:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:area(lastCell="B58")
+jx:each(lastCell="B58" items="rList4" var="r" select="r.transaction=~'^([0-9]{2,2})+_([0-9]{3,3})+_([A-Za-z])+_([A-Za-z])+$' and r.averageResponseTime&gt;30.0")</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>John Mathew</author>
+  </authors>
+  <commentList>
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{DCD0CE34-4CC2-4B15-B2B8-930559608FE8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>John Mathew:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:area(lastCell="L6")
+jx:each(lastCell="L6" items="rList1" var="r" select="r.transaction=~'^([0-9]{2,2})+_([0-9]{3,3})+_([A-Za-z])+_([A-Za-z])+$'")</t>
         </r>
       </text>
     </comment>
@@ -159,7 +269,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>Summary</t>
   </si>
@@ -263,97 +373,10 @@
     <t>Transactions Fall between 10 to 20 Seconds</t>
   </si>
   <si>
-    <t>18_ViewDocuments_003_LoanSummary</t>
-  </si>
-  <si>
-    <t>20_LoanOrderDocs_003_LoanSummary</t>
-  </si>
-  <si>
-    <t>21_OrderAppraisal_003_LoanSummary</t>
-  </si>
-  <si>
-    <t>18_ViewDocuments_004_/documents</t>
-  </si>
-  <si>
-    <t>20_LoanOrderDocs_004_OrderDocs</t>
-  </si>
-  <si>
-    <t>15_LoanConditions_004_Conditions</t>
-  </si>
-  <si>
-    <t>20_LoanOrderDocs_005_OrderDocsSubmit</t>
-  </si>
-  <si>
-    <t>21_OrderAppraisal_004_Account/Logo</t>
-  </si>
-  <si>
-    <t>09_1003Form_014_hudinfo</t>
-  </si>
-  <si>
     <t>Transactions Fall between 20 - 30 seconds</t>
   </si>
   <si>
-    <t>09_1003Form_009_Incomeandexpenses</t>
-  </si>
-  <si>
-    <t>09_1003Form_004_loanUrlaConfig</t>
-  </si>
-  <si>
-    <t>08_LoanSummary_005_Loansummary</t>
-  </si>
-  <si>
-    <t>17_UPLOADDocuments_003_LoanSummary</t>
-  </si>
-  <si>
-    <t>17_UPLOADDocuments_004_UploadDocumens</t>
-  </si>
-  <si>
-    <t>15_LoanConditions_003_LoanSummary</t>
-  </si>
-  <si>
     <t>Transactions Fall beyond 30 seconds</t>
-  </si>
-  <si>
-    <t>09_1003Form_003_LoanSummary</t>
-  </si>
-  <si>
-    <t>09_1003Form_013_hmda</t>
-  </si>
-  <si>
-    <t>09_1003Form_007_Borrowers1003</t>
-  </si>
-  <si>
-    <t>09_1003Form_008_/employment</t>
-  </si>
-  <si>
-    <t>09_1003Form_006_propertyinfo1003</t>
-  </si>
-  <si>
-    <t>09_1003Form_005_loaninfo</t>
-  </si>
-  <si>
-    <t>09_1003Form_012_declaration</t>
-  </si>
-  <si>
-    <t>09_1003Form_011_/urlaTransaction</t>
-  </si>
-  <si>
-    <t>03_Pagenation_Page10,20,30_ActiveLoans_003_pipelineloans</t>
-  </si>
-  <si>
-    <t>10_Pricing_004_Pricing</t>
-  </si>
-  <si>
-    <t>07_RegisterLoan_manualRegistration_004_LoanRegister</t>
-  </si>
-  <si>
-    <t>07_Script2_ManualRegistrationMaxflow_005_/finexpuiapp/api/loans</t>
-  </si>
-  <si>
-    <t>09_1003Form_010_Assetandliability</t>
-  </si>
-  <si>
-    <t>06_RegisterLoan_UploadFNM_003_ /finexploan/api/loans/fnm/3.2</t>
   </si>
   <si>
     <t>Average</t>
@@ -377,7 +400,7 @@
     <t>Std. Dev.</t>
   </si>
   <si>
-    <t>10_Pricing_0+B30:B3703_LoanSummary</t>
+    <t>${r.transaction}</t>
   </si>
 </sst>
 </file>
@@ -1445,8 +1468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK136"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1518,7 +1541,7 @@
         <v>4</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="H11" s="13" t="s">
         <v>5</v>
@@ -5656,16 +5679,16 @@
   <dimension ref="B1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E3" sqref="B3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -5691,7 +5714,7 @@
         <v>18</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="I2" s="11" t="s">
         <v>21</v>
@@ -5726,11 +5749,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E02DFAF2-AB79-423A-ACCB-9EDFD585605A}">
-  <dimension ref="B2:B71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E02DFAF2-AB79-423A-ACCB-9EDFD585605A}">
+  <dimension ref="B2:B69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5751,47 +5774,33 @@
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="10"/>
+      <c r="B5" s="6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
-        <v>65</v>
-      </c>
+      <c r="B6" s="14"/>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
-        <v>27</v>
-      </c>
+      <c r="B7" s="14"/>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
-        <v>28</v>
-      </c>
+      <c r="B8" s="14"/>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
-        <v>29</v>
-      </c>
+      <c r="B9" s="14"/>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="14" t="s">
-        <v>30</v>
-      </c>
+      <c r="B10" s="14"/>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
-        <v>31</v>
-      </c>
+      <c r="B11" s="14"/>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="14" t="s">
-        <v>32</v>
-      </c>
+      <c r="B12" s="14"/>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="14" t="s">
-        <v>33</v>
-      </c>
+      <c r="B13" s="14"/>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
@@ -5834,54 +5843,36 @@
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="14" t="s">
-        <v>65</v>
+      <c r="B30" s="14"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="14" t="s">
-        <v>28</v>
-      </c>
+      <c r="B32" s="14"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="14" t="s">
-        <v>29</v>
-      </c>
+      <c r="B33" s="14"/>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="14" t="s">
-        <v>30</v>
-      </c>
+      <c r="B34" s="14"/>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="14" t="s">
-        <v>31</v>
-      </c>
+      <c r="B35" s="14"/>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="14" t="s">
-        <v>32</v>
-      </c>
+      <c r="B36" s="14"/>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="14" t="s">
-        <v>33</v>
-      </c>
+      <c r="B37" s="14"/>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="14" t="s">
-        <v>34</v>
-      </c>
+      <c r="B38" s="14"/>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="14" t="s">
-        <v>35</v>
-      </c>
+      <c r="B39" s="14"/>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="10"/>
@@ -5894,7 +5885,7 @@
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" s="8" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
@@ -5903,38 +5894,25 @@
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" s="10" t="s">
-        <v>37</v>
+      <c r="B46" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" s="10" t="s">
-        <v>38</v>
-      </c>
+      <c r="B47" s="10"/>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="B48" s="10"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="10" t="s">
-        <v>40</v>
-      </c>
+      <c r="B49" s="10"/>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="6" t="s">
-        <v>42</v>
-      </c>
+      <c r="B50" s="10"/>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" s="8" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
@@ -5943,78 +5921,47 @@
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B58" s="10" t="s">
-        <v>44</v>
+      <c r="B58" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B59" s="10" t="s">
-        <v>45</v>
-      </c>
+      <c r="B59" s="10"/>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B60" s="10" t="s">
-        <v>46</v>
-      </c>
+      <c r="B60" s="10"/>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B61" s="10" t="s">
-        <v>47</v>
-      </c>
+      <c r="B61" s="10"/>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B62" s="10" t="s">
-        <v>48</v>
-      </c>
+      <c r="B62" s="10"/>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B63" s="10" t="s">
-        <v>49</v>
-      </c>
+      <c r="B63" s="10"/>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B64" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="B64" s="10"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="10" t="s">
-        <v>51</v>
-      </c>
+      <c r="B65" s="10"/>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="10" t="s">
-        <v>52</v>
-      </c>
+      <c r="B66" s="10"/>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="10" t="s">
-        <v>53</v>
-      </c>
+      <c r="B67" s="10"/>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="69" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B69" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="6" t="s">
-        <v>57</v>
-      </c>
+      <c r="B68" s="10"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6022,8 +5969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F365DCCC-F353-4CFC-BF73-ACC82FEB2F4F}">
   <dimension ref="B4:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6045,25 +5992,25 @@
         <v>16</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>18</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="I5" s="16" t="s">
         <v>21</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="K5" s="17" t="s">
         <v>23</v>
@@ -6073,8 +6020,8 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>

</xml_diff>

<commit_message>
Bettered Template for highlighting transactions in API Level sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/template/Jmeter_Reporting_Template.xlsx
+++ b/src/test/resources/template/Jmeter_Reporting_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john.mathew\workspace_oxygen\meagan\src\test\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113B413D-3909-4C95-9EED-89D755B1F3C3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBC514B-A633-4EE7-A0B7-3757D00E3799}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transaction Level" sheetId="1" r:id="rId1"/>
@@ -114,8 +114,9 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="L3")
-jx:each(lastCell="L3" items="rList2" var="r")</t>
+jx:area(lastCell="L4")
+jx:each(lastCell="L4" items="rList2" var="r")
+jx:if(condition="r.transaction=~'^([0-9]{2,2})+_([0-9]{3,3})+_([A-Za-z])+_([A-Za-z])+$'"  lastCell="L4"  areas=["B3:L3","B4:L4"])</t>
         </r>
       </text>
     </comment>
@@ -1062,7 +1063,7 @@
     <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -1103,6 +1104,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="14" xfId="41" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="56">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -1468,7 +1470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -5678,8 +5680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170E5F5C-ECD9-4726-9276-F98E37AE34A1}">
   <dimension ref="B1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="B3:E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5730,7 +5732,7 @@
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="7"/>
+      <c r="B3" s="24"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>

</xml_diff>

<commit_message>
Fixed issues with template
</commit_message>
<xml_diff>
--- a/src/test/resources/template/Jmeter_Reporting_Template.xlsx
+++ b/src/test/resources/template/Jmeter_Reporting_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john.mathew\workspace_oxygen\meagan\src\test\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBC514B-A633-4EE7-A0B7-3757D00E3799}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F01DE18-46B2-44BC-BB39-59FB7CB39F97}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
           </rPr>
           <t xml:space="preserve">
 jx:area(lastCell="L12")
-jx:each(lastCell="L12" items="rList1" var="r" select="r.transaction=~'^([0-9]{2,2})+_([0-9]{3,3})+_([A-Za-z])+_([A-Za-z])+$'")</t>
+jx:each(lastCell="L12" items="rList1" var="r" select="r.transaction=~'^([0-9]{2,2})+_([0-9]{3,3})+(_([A-Za-z])+)+_([A-Za-z])+$'")</t>
         </r>
       </text>
     </comment>
@@ -116,7 +116,7 @@
           <t xml:space="preserve">
 jx:area(lastCell="L4")
 jx:each(lastCell="L4" items="rList2" var="r")
-jx:if(condition="r.transaction=~'^([0-9]{2,2})+_([0-9]{3,3})+_([A-Za-z])+_([A-Za-z])+$'"  lastCell="L4"  areas=["B3:L3","B4:L4"])</t>
+jx:if(condition="r.transaction=~'^([0-9]{2,2})+_([0-9]{3,3})+(_([A-Za-z])+)+_([A-Za-z])+$'"  lastCell="L4"  areas=["B3:L3","B4:L4"])</t>
         </r>
       </text>
     </comment>
@@ -151,7 +151,7 @@
           </rPr>
           <t xml:space="preserve">
 jx:area(lastCell="B5")
-jx:each(lastCell="B5" items="rList4" var="r" select="r.transaction=~'^([0-9]{2,2})+_([0-9]{3,3})+_([A-Za-z])+_([A-Za-z])+$' and r.averageResponseTime&gt;=5.0 and r.averageResponseTime&lt;10.0")</t>
+jx:each(lastCell="B5" items="rList4" var="r" select="r.transaction=~'^([0-9]{2,2})+_([0-9]{3,3})+(_([A-Za-z])+)+_([A-Za-z])+$' and r.averageResponseTime&gt;=5.0 and r.averageResponseTime&lt;10.0")</t>
         </r>
       </text>
     </comment>
@@ -176,7 +176,7 @@
           </rPr>
           <t xml:space="preserve">
 jx:area(lastCell="B31")
-jx:each(lastCell="B31" items="rList4" var="r" select="r.transaction=~'^([0-9]{2,2})+_([0-9]{3,3})+_([A-Za-z])+_([A-Za-z])+$' and r.averageResponseTime&gt;=10.0 and r.averageResponseTime&lt;20.0")</t>
+jx:each(lastCell="B31" items="rList4" var="r" select="r.transaction=~'^([0-9]{2,2})+_([0-9]{3,3})+(_([A-Za-z])+)+_([A-Za-z])+$' and r.averageResponseTime&gt;=10.0 and r.averageResponseTime&lt;20.0")</t>
         </r>
       </text>
     </comment>
@@ -201,7 +201,7 @@
           </rPr>
           <t xml:space="preserve">
 jx:area(lastCell="B46")
-jx:each(lastCell="B46" items="rList4" var="r" select="r.transaction=~'^([0-9]{2,2})+_([0-9]{3,3})+_([A-Za-z])+_([A-Za-z])+$' and r.averageResponseTime&gt;=20.0 and r.averageResponseTime&lt;30.0")</t>
+jx:each(lastCell="B46" items="rList4" var="r" select="r.transaction=~'^([0-9]{2,2})+_([0-9]{3,3})+(_([A-Za-z])+)+_([A-Za-z])+$' and r.averageResponseTime&gt;=20.0 and r.averageResponseTime&lt;30.0")</t>
         </r>
       </text>
     </comment>
@@ -226,7 +226,7 @@
           </rPr>
           <t xml:space="preserve">
 jx:area(lastCell="B58")
-jx:each(lastCell="B58" items="rList4" var="r" select="r.transaction=~'^([0-9]{2,2})+_([0-9]{3,3})+_([A-Za-z])+_([A-Za-z])+$' and r.averageResponseTime&gt;30.0")</t>
+jx:each(lastCell="B58" items="rList4" var="r" select="r.transaction=~'^([0-9]{2,2})+_([0-9]{3,3})+(_([A-Za-z])+)+_([A-Za-z])+$' and r.averageResponseTime&gt;30.0")</t>
         </r>
       </text>
     </comment>
@@ -261,7 +261,7 @@
           </rPr>
           <t xml:space="preserve">
 jx:area(lastCell="L6")
-jx:each(lastCell="L6" items="rList1" var="r" select="r.transaction=~'^([0-9]{2,2})+_([0-9]{3,3})+_([A-Za-z])+_([A-Za-z])+$'")</t>
+jx:each(lastCell="L6" items="rList3" var="r" select="r.transaction=~'^([0-9]{2,2})+_([0-9]{3,3})+(_([A-Za-z])+)+_([A-Za-z])+$'")</t>
         </r>
       </text>
     </comment>
@@ -270,7 +270,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>Summary</t>
   </si>
@@ -344,40 +344,7 @@
     <t>KB/sec</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Transactions Fall between 5 to 10 Seconds</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
     <t>=====================================</t>
-  </si>
-  <si>
-    <t>Transactions Fall between 10 to 20 Seconds</t>
-  </si>
-  <si>
-    <t>Transactions Fall between 20 - 30 seconds</t>
-  </si>
-  <si>
-    <t>Transactions Fall beyond 30 seconds</t>
   </si>
   <si>
     <t>Average</t>
@@ -401,7 +368,37 @@
     <t>Std. Dev.</t>
   </si>
   <si>
-    <t>${r.transaction}</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Transactions Falling between 5 to 10 Seconds</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Transactions Falling between 10 to 20 Seconds</t>
+  </si>
+  <si>
+    <t>Transactions Falling beyond 30 seconds</t>
+  </si>
+  <si>
+    <t>Transactions Falling between 20 to 30 seconds</t>
   </si>
 </sst>
 </file>
@@ -1104,7 +1101,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="14" xfId="41" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="14" xfId="20" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="56">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -1543,7 +1540,7 @@
         <v>4</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H11" s="13" t="s">
         <v>5</v>
@@ -5678,7 +5675,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170E5F5C-ECD9-4726-9276-F98E37AE34A1}">
-  <dimension ref="B1:L3"/>
+  <dimension ref="B1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -5716,7 +5713,7 @@
         <v>18</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I2" s="11" t="s">
         <v>21</v>
@@ -5744,6 +5741,19 @@
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
     </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -5754,8 +5764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E02DFAF2-AB79-423A-ACCB-9EDFD585605A}">
   <dimension ref="B2:B69"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5767,19 +5777,15 @@
   <sheetData>
     <row r="2" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25"/>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="14"/>
     </row>
@@ -5836,22 +5842,18 @@
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="14"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25"/>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" s="14"/>
     </row>
@@ -5887,19 +5889,15 @@
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" s="8" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25"/>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" s="10"/>
     </row>
@@ -5914,19 +5912,15 @@
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" s="8" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B58" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25"/>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="10"/>
     </row>
@@ -5971,7 +5965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F365DCCC-F353-4CFC-BF73-ACC82FEB2F4F}">
   <dimension ref="B4:L14"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6:E6"/>
     </sheetView>
   </sheetViews>
@@ -5994,25 +5988,25 @@
         <v>16</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>18</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I5" s="16" t="s">
         <v>21</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="K5" s="17" t="s">
         <v>23</v>

</xml_diff>